<commit_message>
Analysis update: - Calibration - Plot raw data all runs - Logbook
</commit_message>
<xml_diff>
--- a/RBS_21Janeiro/Logbook-RBS_21Janeiro.xlsx
+++ b/RBS_21Janeiro/Logbook-RBS_21Janeiro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Runs" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="90">
   <si>
     <t>2000 keV</t>
   </si>
@@ -421,7 +421,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,6 +614,12 @@
         <bgColor rgb="FFDAE3F3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="32">
     <border>
@@ -1012,7 +1018,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="212">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1611,6 +1617,7 @@
     <xf numFmtId="0" fontId="0" fillId="29" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1931,11 +1938,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="4098608"/>
-        <c:axId val="4111120"/>
+        <c:axId val="-1781517584"/>
+        <c:axId val="-1781511600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4098608"/>
+        <c:axId val="-1781517584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2013,12 +2020,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4111120"/>
+        <c:crossAx val="-1781511600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4111120"/>
+        <c:axId val="-1781511600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2096,7 +2103,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4098608"/>
+        <c:crossAx val="-1781517584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2315,7 +2322,7 @@
             <c:numRef>
               <c:f>('[1]Ta-Nb-V Calib - RBS1 - Alfa'!$R$16,'[1]Ta-Nb-V Calib - RBS1 - Alfa'!$R$21,'[1]Ta-Nb-V Calib - RBS1 - Alfa'!$R$26)</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>954.79088945786589</c:v>
@@ -2339,11 +2346,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="4102416"/>
-        <c:axId val="4107856"/>
+        <c:axId val="-1781509424"/>
+        <c:axId val="-1781511056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4102416"/>
+        <c:axId val="-1781509424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2424,12 +2431,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="4107856"/>
+        <c:crossAx val="-1781511056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4107856"/>
+        <c:axId val="-1781511056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2510,7 +2517,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2547,7 +2554,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4102416"/>
+        <c:crossAx val="-1781509424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3230,7 +3237,7 @@
       <sheetName val="Ta-Nb-V Calib - RBS1 - Protoes"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="I2">
@@ -3293,7 +3300,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3564,8 +3571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3695,8 +3702,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>21</v>
+      <c r="A7" s="212">
+        <v>1</v>
       </c>
       <c r="B7" s="25">
         <v>4</v>
@@ -3736,6 +3743,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="212">
+        <v>1</v>
+      </c>
       <c r="B9" s="26">
         <v>6</v>
       </c>
@@ -3770,6 +3780,9 @@
       <c r="H10" s="27"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="212">
+        <v>1</v>
+      </c>
       <c r="B11" s="27">
         <v>8</v>
       </c>
@@ -3812,6 +3825,9 @@
       <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="212">
+        <v>1</v>
+      </c>
       <c r="B13" s="47">
         <v>10</v>
       </c>
@@ -3895,7 +3911,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" s="212"/>
       <c r="B17" s="30">
         <v>13</v>
       </c>
@@ -3920,7 +3937,7 @@
       <c r="I17" s="6"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B18" s="31">
         <v>14</v>
       </c>
@@ -3943,7 +3960,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="212"/>
       <c r="B19" s="32">
         <v>15</v>
       </c>
@@ -3958,7 +3976,7 @@
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B20" s="55">
         <v>16</v>
       </c>
@@ -3975,7 +3993,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" s="212"/>
       <c r="B21" s="58">
         <v>17</v>
       </c>
@@ -3992,7 +4011,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="212"/>
       <c r="B22" s="62">
         <v>18</v>
       </c>
@@ -4011,7 +4031,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B23" s="66">
         <v>19</v>
       </c>
@@ -4030,7 +4050,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="212"/>
       <c r="B24" s="69">
         <v>20</v>
       </c>
@@ -4068,8 +4089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="AC59" sqref="AC59"/>
+    <sheetView topLeftCell="A19" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5884,7 +5905,7 @@
       <c r="Y27" s="163"/>
       <c r="Z27" s="164"/>
       <c r="AA27" s="165">
-        <f t="shared" ref="AA26:AA27" si="31">(Y27-Z27)*2.381</f>
+        <f t="shared" ref="AA27" si="31">(Y27-Z27)*2.381</f>
         <v>0</v>
       </c>
       <c r="AB27" s="166">
@@ -5915,7 +5936,7 @@
       <c r="AL27" s="177"/>
       <c r="AM27" s="178"/>
       <c r="AN27" s="165">
-        <f t="shared" ref="AN26:AN27" si="34">(AL27-AM27)*2.381</f>
+        <f t="shared" ref="AN27" si="34">(AL27-AM27)*2.381</f>
         <v>0</v>
       </c>
       <c r="AO27" s="166">
@@ -6532,7 +6553,7 @@
       <c r="Y44" s="163"/>
       <c r="Z44" s="164"/>
       <c r="AA44" s="165">
-        <f t="shared" ref="AA44:AA45" si="37">(Y44-Z44)*2.381</f>
+        <f t="shared" ref="AA44" si="37">(Y44-Z44)*2.381</f>
         <v>0</v>
       </c>
       <c r="AB44" s="166">
@@ -6563,7 +6584,7 @@
       <c r="AL44" s="177"/>
       <c r="AM44" s="178"/>
       <c r="AN44" s="165">
-        <f t="shared" ref="AN44:AN45" si="40">(AL44-AM44)*2.381</f>
+        <f t="shared" ref="AN44" si="40">(AL44-AM44)*2.381</f>
         <v>0</v>
       </c>
       <c r="AO44" s="166">
@@ -6823,7 +6844,7 @@
       </c>
       <c r="Z50" s="164"/>
       <c r="AA50" s="165">
-        <f t="shared" ref="AA50:AA51" si="43">(Y50-Z50)*2.381</f>
+        <f t="shared" ref="AA50" si="43">(Y50-Z50)*2.381</f>
         <v>1526.2209999999998</v>
       </c>
       <c r="AB50" s="166">
@@ -6856,7 +6877,7 @@
       </c>
       <c r="AM50" s="178"/>
       <c r="AN50" s="165">
-        <f t="shared" ref="AN50:AN51" si="46">(AL50-AM50)*2.381</f>
+        <f t="shared" ref="AN50" si="46">(AL50-AM50)*2.381</f>
         <v>1402.4089999999999</v>
       </c>
       <c r="AO50" s="166">

</xml_diff>

<commit_message>
RBS from 21 Jan analysis
</commit_message>
<xml_diff>
--- a/RBS_21Janeiro/Logbook-RBS_21Janeiro.xlsx
+++ b/RBS_21Janeiro/Logbook-RBS_21Janeiro.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Runs" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="91">
   <si>
     <t>2000 keV</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>35 mm</t>
+  </si>
+  <si>
+    <t>Cu</t>
   </si>
 </sst>
 </file>
@@ -1938,11 +1941,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1781517584"/>
-        <c:axId val="-1781511600"/>
+        <c:axId val="80584976"/>
+        <c:axId val="80583888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1781517584"/>
+        <c:axId val="80584976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2020,12 +2023,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1781511600"/>
+        <c:crossAx val="80583888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1781511600"/>
+        <c:axId val="80583888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2103,7 +2106,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1781517584"/>
+        <c:crossAx val="80584976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2152,7 +2155,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2322,7 +2324,7 @@
             <c:numRef>
               <c:f>('[1]Ta-Nb-V Calib - RBS1 - Alfa'!$R$16,'[1]Ta-Nb-V Calib - RBS1 - Alfa'!$R$21,'[1]Ta-Nb-V Calib - RBS1 - Alfa'!$R$26)</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>954.79088945786589</c:v>
@@ -2346,11 +2348,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1781509424"/>
-        <c:axId val="-1781511056"/>
+        <c:axId val="80590416"/>
+        <c:axId val="80586064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1781509424"/>
+        <c:axId val="80590416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2431,12 +2433,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1781511056"/>
+        <c:crossAx val="80586064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1781511056"/>
+        <c:axId val="80586064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2487,7 +2489,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2517,7 +2518,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2554,7 +2555,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1781509424"/>
+        <c:crossAx val="80590416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3571,8 +3572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4089,8 +4090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4184,7 +4185,7 @@
         <v>15.999000000000001</v>
       </c>
       <c r="F4" s="86">
-        <f t="shared" ref="F4:F11" si="0">((SQRT(1-(1/E4)^2*SIN(RADIANS(165))^2)+1/E4*COS(RADIANS(165)))/(1+1/E4))^2</f>
+        <f t="shared" ref="F4:F12" si="0">((SQRT(1-(1/E4)^2*SIN(RADIANS(165))^2)+1/E4*COS(RADIANS(165)))/(1+1/E4))^2</f>
         <v>0.78185798881983415</v>
       </c>
       <c r="G4" s="87">
@@ -4432,7 +4433,7 @@
         <v>0.9812026480871997</v>
       </c>
       <c r="G9" s="130">
-        <f t="shared" ref="G9:G11" si="5">$B$1*F9</f>
+        <f t="shared" ref="G9:G12" si="5">$B$1*F9</f>
         <v>1962.4052961743994</v>
       </c>
       <c r="H9" s="131">
@@ -4669,6 +4670,27 @@
       <c r="AV11" s="156"/>
     </row>
     <row r="12" spans="1:48" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12">
+        <v>29</v>
+      </c>
+      <c r="E12">
+        <v>63.545999999999999</v>
+      </c>
+      <c r="F12" s="204">
+        <f t="shared" si="0"/>
+        <v>0.93999634329545045</v>
+      </c>
+      <c r="G12" s="205">
+        <f t="shared" si="5"/>
+        <v>1879.9926865909008</v>
+      </c>
+      <c r="H12" s="208">
+        <f>(G12-46.367)/2.3671</f>
+        <v>774.62958328372304</v>
+      </c>
       <c r="K12" s="162" t="s">
         <v>70</v>
       </c>

</xml_diff>